<commit_message>
Erro identificado, Santos não está mais na liga principal.
</commit_message>
<xml_diff>
--- a/Times-br.xlsx
+++ b/Times-br.xlsx
@@ -54,9 +54,6 @@
     <t>SÃO PAULO</t>
   </si>
   <si>
-    <t>SANTOS</t>
-  </si>
-  <si>
     <t>BRAGANTINO</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>ATLÉTICO MG</t>
+  </si>
+  <si>
+    <t>ATHLETICO PR</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1098,25 +1098,25 @@
     </row>
     <row r="8" spans="1:5" ht="15.75">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>38</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>21</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>24</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>33</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75">
       <c r="A14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>50</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
         <v>30</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
         <v>13</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1">
         <v>18</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75">
       <c r="A19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1">
         <v>46</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>38</v>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75">
       <c r="A21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>49</v>

</xml_diff>